<commit_message>
changed filling zhr_vh.xslx for new order (22/03/2022) - end
</commit_message>
<xml_diff>
--- a/Excell/zhr_ozhr.xlsx
+++ b/Excell/zhr_ozhr.xlsx
@@ -3,32 +3,34 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DE9C32-DF16-4433-9806-FE32B3D35B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A586D7-1B0F-4682-BEF5-1EF6FDF2D15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1095" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="L1" sheetId="1" r:id="rId1"/>
-    <sheet name="Part 1" sheetId="3" r:id="rId2"/>
-    <sheet name="Part 2" sheetId="4" r:id="rId3"/>
-    <sheet name="Part 3" sheetId="5" r:id="rId4"/>
-    <sheet name="Part 4" sheetId="6" r:id="rId5"/>
-    <sheet name="Part 5" sheetId="7" r:id="rId6"/>
-    <sheet name="Part 6" sheetId="8" r:id="rId7"/>
-    <sheet name="Part 7" sheetId="9" r:id="rId8"/>
-    <sheet name="L2" sheetId="2" r:id="rId9"/>
+    <sheet name="L_tittle" sheetId="10" r:id="rId1"/>
+    <sheet name="L1" sheetId="1" r:id="rId2"/>
+    <sheet name="Part 1" sheetId="3" r:id="rId3"/>
+    <sheet name="Part 2" sheetId="4" r:id="rId4"/>
+    <sheet name="Part 3" sheetId="5" r:id="rId5"/>
+    <sheet name="Part 4" sheetId="6" r:id="rId6"/>
+    <sheet name="Part 5" sheetId="7" r:id="rId7"/>
+    <sheet name="Part 6" sheetId="8" r:id="rId8"/>
+    <sheet name="Part 7" sheetId="9" r:id="rId9"/>
+    <sheet name="L2" sheetId="2" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Part 1'!$A:$E,'Part 1'!$1:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Part 2'!$A:$E,'Part 2'!$1:$5</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Part 3'!$A:$C,'Part 3'!$1:$5</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'Part 6'!$A:$B,'Part 6'!$1:$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Part 1'!$A$1:$E$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Part 2'!$A$1:$E$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Part 3'!$A$1:$C$25</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Part 4'!$A$1:$E$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'Part 6'!$A$1:$B$21</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">'Part 7'!$A$1:$E$46</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Part 1'!$A:$E,'Part 1'!$1:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Part 2'!$A:$E,'Part 2'!$1:$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'Part 3'!$A:$C,'Part 3'!$1:$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">'Part 6'!$A:$B,'Part 6'!$1:$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">L_tittle!$A$1:$L$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Part 1'!$A$1:$E$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Part 2'!$A$1:$E$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Part 3'!$A$1:$C$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Part 4'!$A$1:$E$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'Part 6'!$A$1:$B$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'Part 7'!$A$1:$E$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="190">
   <si>
     <t>Застройщик</t>
   </si>
@@ -701,12 +703,30 @@
   <si>
     <t>table_6</t>
   </si>
+  <si>
+    <t>от км</t>
+  </si>
+  <si>
+    <t>до км</t>
+  </si>
+  <si>
+    <t>до ПК</t>
+  </si>
+  <si>
+    <t>от ПК</t>
+  </si>
+  <si>
+    <t>Окончание работ:</t>
+  </si>
+  <si>
+    <t>Начало работ:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -931,6 +951,13 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1084,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1436,6 +1463,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1774,11 +1810,745 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4DFC98B-EF2D-41DF-886E-6F404262C6D5}">
+  <dimension ref="A1:L46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="12" width="7.28515625" customWidth="1"/>
+    <col min="13" max="21" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="1:12" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="144" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" s="144"/>
+      <c r="C19" s="144"/>
+      <c r="D19" s="144"/>
+      <c r="E19" s="144"/>
+      <c r="F19" s="144"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="144"/>
+      <c r="I19" s="144"/>
+      <c r="J19" s="144"/>
+      <c r="K19" s="144"/>
+      <c r="L19" s="18"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="145">
+        <f>L_tittle!R1</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="145"/>
+      <c r="D22" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="H22" s="145">
+        <f>R2</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="145"/>
+      <c r="J22" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="146">
+        <f>'L1'!A3</f>
+        <v>0</v>
+      </c>
+      <c r="B24" s="146"/>
+      <c r="C24" s="146"/>
+      <c r="D24" s="146"/>
+      <c r="E24" s="146"/>
+      <c r="F24" s="146"/>
+      <c r="G24" s="146"/>
+      <c r="H24" s="146"/>
+      <c r="I24" s="146"/>
+      <c r="J24" s="146"/>
+      <c r="K24" s="146"/>
+      <c r="L24" s="146"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="146"/>
+      <c r="B25" s="146"/>
+      <c r="C25" s="146"/>
+      <c r="D25" s="146"/>
+      <c r="E25" s="146"/>
+      <c r="F25" s="146"/>
+      <c r="G25" s="146"/>
+      <c r="H25" s="146"/>
+      <c r="I25" s="146"/>
+      <c r="J25" s="146"/>
+      <c r="K25" s="146"/>
+      <c r="L25" s="146"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="146"/>
+      <c r="B26" s="146"/>
+      <c r="C26" s="146"/>
+      <c r="D26" s="146"/>
+      <c r="E26" s="146"/>
+      <c r="F26" s="146"/>
+      <c r="G26" s="146"/>
+      <c r="H26" s="146"/>
+      <c r="I26" s="146"/>
+      <c r="J26" s="146"/>
+      <c r="K26" s="146"/>
+      <c r="L26" s="146"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="145">
+        <f>R3</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="145"/>
+      <c r="K43" s="145"/>
+      <c r="L43" s="18"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="145">
+        <f>R4</f>
+        <v>0</v>
+      </c>
+      <c r="J45" s="145"/>
+      <c r="K45" s="145"/>
+      <c r="L45" s="18"/>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="A24:L26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="87" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC142"/>
+  <dimension ref="A1:AC144"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A118" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30:Y30"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A85" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="L137" sqref="L137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -4796,66 +5566,66 @@
       <c r="AC139" s="75"/>
     </row>
     <row r="140" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A140" s="77"/>
-      <c r="B140" s="78"/>
-      <c r="C140" s="79"/>
-      <c r="D140" s="78"/>
-      <c r="E140" s="77"/>
-      <c r="F140" s="80"/>
-      <c r="G140" s="80"/>
-      <c r="H140" s="80"/>
-      <c r="I140" s="78"/>
-      <c r="J140" s="77"/>
-      <c r="K140" s="80"/>
-      <c r="L140" s="80"/>
-      <c r="M140" s="80"/>
-      <c r="N140" s="80"/>
-      <c r="O140" s="80"/>
-      <c r="P140" s="80"/>
-      <c r="Q140" s="80"/>
-      <c r="R140" s="80"/>
-      <c r="S140" s="80"/>
-      <c r="T140" s="80"/>
-      <c r="U140" s="80"/>
-      <c r="V140" s="80"/>
-      <c r="W140" s="80"/>
-      <c r="X140" s="78"/>
-      <c r="Y140" s="79"/>
-      <c r="Z140" s="81"/>
-      <c r="AA140" s="80"/>
-      <c r="AB140" s="80"/>
-      <c r="AC140" s="78"/>
+      <c r="A140" s="74"/>
+      <c r="B140" s="75"/>
+      <c r="C140" s="74"/>
+      <c r="D140" s="75"/>
+      <c r="E140" s="76"/>
+      <c r="F140" s="33"/>
+      <c r="G140" s="33"/>
+      <c r="H140" s="33"/>
+      <c r="I140" s="75"/>
+      <c r="J140" s="76"/>
+      <c r="K140" s="33"/>
+      <c r="L140" s="33"/>
+      <c r="M140" s="33"/>
+      <c r="N140" s="33"/>
+      <c r="O140" s="33"/>
+      <c r="P140" s="33"/>
+      <c r="Q140" s="33"/>
+      <c r="R140" s="33"/>
+      <c r="S140" s="33"/>
+      <c r="T140" s="33"/>
+      <c r="U140" s="33"/>
+      <c r="V140" s="33"/>
+      <c r="W140" s="33"/>
+      <c r="X140" s="75"/>
+      <c r="Y140" s="74"/>
+      <c r="Z140" s="33"/>
+      <c r="AA140" s="33"/>
+      <c r="AB140" s="33"/>
+      <c r="AC140" s="75"/>
     </row>
     <row r="141" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A141" s="77"/>
-      <c r="B141" s="78"/>
-      <c r="C141" s="79"/>
-      <c r="D141" s="78"/>
-      <c r="E141" s="77"/>
-      <c r="F141" s="80"/>
-      <c r="G141" s="80"/>
-      <c r="H141" s="80"/>
-      <c r="I141" s="78"/>
-      <c r="J141" s="77"/>
-      <c r="K141" s="80"/>
-      <c r="L141" s="80"/>
-      <c r="M141" s="80"/>
-      <c r="N141" s="80"/>
-      <c r="O141" s="80"/>
-      <c r="P141" s="80"/>
-      <c r="Q141" s="80"/>
-      <c r="R141" s="80"/>
-      <c r="S141" s="80"/>
-      <c r="T141" s="80"/>
-      <c r="U141" s="80"/>
-      <c r="V141" s="80"/>
-      <c r="W141" s="80"/>
-      <c r="X141" s="78"/>
-      <c r="Y141" s="79"/>
-      <c r="Z141" s="81"/>
-      <c r="AA141" s="80"/>
-      <c r="AB141" s="80"/>
-      <c r="AC141" s="78"/>
+      <c r="A141" s="74"/>
+      <c r="B141" s="75"/>
+      <c r="C141" s="74"/>
+      <c r="D141" s="75"/>
+      <c r="E141" s="76"/>
+      <c r="F141" s="33"/>
+      <c r="G141" s="33"/>
+      <c r="H141" s="33"/>
+      <c r="I141" s="75"/>
+      <c r="J141" s="76"/>
+      <c r="K141" s="33"/>
+      <c r="L141" s="33"/>
+      <c r="M141" s="33"/>
+      <c r="N141" s="33"/>
+      <c r="O141" s="33"/>
+      <c r="P141" s="33"/>
+      <c r="Q141" s="33"/>
+      <c r="R141" s="33"/>
+      <c r="S141" s="33"/>
+      <c r="T141" s="33"/>
+      <c r="U141" s="33"/>
+      <c r="V141" s="33"/>
+      <c r="W141" s="33"/>
+      <c r="X141" s="75"/>
+      <c r="Y141" s="74"/>
+      <c r="Z141" s="33"/>
+      <c r="AA141" s="33"/>
+      <c r="AB141" s="33"/>
+      <c r="AC141" s="75"/>
     </row>
     <row r="142" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A142" s="77"/>
@@ -4887,6 +5657,68 @@
       <c r="AA142" s="80"/>
       <c r="AB142" s="80"/>
       <c r="AC142" s="78"/>
+    </row>
+    <row r="143" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A143" s="77"/>
+      <c r="B143" s="78"/>
+      <c r="C143" s="79"/>
+      <c r="D143" s="78"/>
+      <c r="E143" s="77"/>
+      <c r="F143" s="80"/>
+      <c r="G143" s="80"/>
+      <c r="H143" s="80"/>
+      <c r="I143" s="78"/>
+      <c r="J143" s="77"/>
+      <c r="K143" s="80"/>
+      <c r="L143" s="80"/>
+      <c r="M143" s="80"/>
+      <c r="N143" s="80"/>
+      <c r="O143" s="80"/>
+      <c r="P143" s="80"/>
+      <c r="Q143" s="80"/>
+      <c r="R143" s="80"/>
+      <c r="S143" s="80"/>
+      <c r="T143" s="80"/>
+      <c r="U143" s="80"/>
+      <c r="V143" s="80"/>
+      <c r="W143" s="80"/>
+      <c r="X143" s="78"/>
+      <c r="Y143" s="79"/>
+      <c r="Z143" s="81"/>
+      <c r="AA143" s="80"/>
+      <c r="AB143" s="80"/>
+      <c r="AC143" s="78"/>
+    </row>
+    <row r="144" spans="1:29" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A144" s="77"/>
+      <c r="B144" s="78"/>
+      <c r="C144" s="79"/>
+      <c r="D144" s="78"/>
+      <c r="E144" s="77"/>
+      <c r="F144" s="80"/>
+      <c r="G144" s="80"/>
+      <c r="H144" s="80"/>
+      <c r="I144" s="78"/>
+      <c r="J144" s="77"/>
+      <c r="K144" s="80"/>
+      <c r="L144" s="80"/>
+      <c r="M144" s="80"/>
+      <c r="N144" s="80"/>
+      <c r="O144" s="80"/>
+      <c r="P144" s="80"/>
+      <c r="Q144" s="80"/>
+      <c r="R144" s="80"/>
+      <c r="S144" s="80"/>
+      <c r="T144" s="80"/>
+      <c r="U144" s="80"/>
+      <c r="V144" s="80"/>
+      <c r="W144" s="80"/>
+      <c r="X144" s="78"/>
+      <c r="Y144" s="79"/>
+      <c r="Z144" s="81"/>
+      <c r="AA144" s="80"/>
+      <c r="AB144" s="80"/>
+      <c r="AC144" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="63">
@@ -4959,7 +5791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
@@ -5222,11 +6054,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -5401,7 +6233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -5564,7 +6396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
@@ -5902,7 +6734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
@@ -6268,7 +7100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -6387,7 +7219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
@@ -6775,37 +7607,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D1" s="87" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>